<commit_message>
add all new file
</commit_message>
<xml_diff>
--- a/resources/Files/ExcelReader.xlsx
+++ b/resources/Files/ExcelReader.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Passwrod</t>
-  </si>
-  <si>
     <t>torikraju</t>
   </si>
   <si>
@@ -47,6 +44,15 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>imat0rik</t>
+  </si>
+  <si>
+    <t>Test_new</t>
   </si>
 </sst>
 </file>
@@ -410,17 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.62109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -431,32 +437,32 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>